<commit_message>
pushing finalized post page
</commit_message>
<xml_diff>
--- a/narrative project/policy_div_names.xlsx
+++ b/narrative project/policy_div_names.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sethschimmel/Documents/GitHub/Interactive-Data-Vis-Sp2020/narrative project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8828A40D-4440-894D-B467-5EE9AD6CADDD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FCAE271-362C-0940-B5B9-1912704D9BA9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="560" windowWidth="27640" windowHeight="16940" xr2:uid="{053DBD3B-D0E5-C14F-85E5-51FCF2FEE08D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="77">
   <si>
     <t>type</t>
   </si>
@@ -252,6 +252,15 @@
   </si>
   <si>
     <t>'Anti-Disinformation Measures': '#disinfo',</t>
+  </si>
+  <si>
+    <t>South Asia</t>
+  </si>
+  <si>
+    <t>Europe &amp; Central Asia</t>
+  </si>
+  <si>
+    <t>Latin America &amp; Caribbean</t>
   </si>
 </sst>
 </file>
@@ -603,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7B6C7EA-29FF-3944-9014-B66ACC5C7E63}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="228" zoomScaleNormal="228" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3:O20"/>
+    <sheetView tabSelected="1" topLeftCell="E13" zoomScale="134" zoomScaleNormal="228" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23:K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1020,6 +1029,222 @@
         <v>73</v>
       </c>
     </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I23" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" t="s">
+        <v>74</v>
+      </c>
+      <c r="K23" t="str">
+        <f>CONCATENATE("'",I23,"': '",J23,"',")</f>
+        <v>'#health_monitor': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K24" t="str">
+        <f t="shared" ref="K24:K40" si="2">CONCATENATE("'",I24,"': '",J24,"',")</f>
+        <v>'#public_aw': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I25" t="s">
+        <v>40</v>
+      </c>
+      <c r="J25" t="s">
+        <v>76</v>
+      </c>
+      <c r="K25" t="str">
+        <f t="shared" si="2"/>
+        <v>'#other_pol': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" t="s">
+        <v>74</v>
+      </c>
+      <c r="K26" t="str">
+        <f t="shared" si="2"/>
+        <v>'#health_rsrc': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I27" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" t="s">
+        <v>75</v>
+      </c>
+      <c r="K27" t="str">
+        <f t="shared" si="2"/>
+        <v>'#task_fc': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I28" t="s">
+        <v>43</v>
+      </c>
+      <c r="J28" t="s">
+        <v>76</v>
+      </c>
+      <c r="K28" t="str">
+        <f t="shared" si="2"/>
+        <v>'#ext_border': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I29" t="s">
+        <v>44</v>
+      </c>
+      <c r="J29" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" t="str">
+        <f t="shared" si="2"/>
+        <v>'#int_border': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" t="str">
+        <f t="shared" si="2"/>
+        <v>'#mass_gath': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" t="s">
+        <v>76</v>
+      </c>
+      <c r="K31" t="str">
+        <f t="shared" si="2"/>
+        <v>'#gov_serv': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>47</v>
+      </c>
+      <c r="J32" t="s">
+        <v>74</v>
+      </c>
+      <c r="K32" t="str">
+        <f t="shared" si="2"/>
+        <v>'#emergency': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="33" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>48</v>
+      </c>
+      <c r="J33" t="s">
+        <v>75</v>
+      </c>
+      <c r="K33" t="str">
+        <f t="shared" si="2"/>
+        <v>'#schools': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="34" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>49</v>
+      </c>
+      <c r="J34" t="s">
+        <v>76</v>
+      </c>
+      <c r="K34" t="str">
+        <f t="shared" si="2"/>
+        <v>'#business': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
+    <row r="35" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>50</v>
+      </c>
+      <c r="J35" t="s">
+        <v>74</v>
+      </c>
+      <c r="K35" t="str">
+        <f t="shared" si="2"/>
+        <v>'#health_test': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>51</v>
+      </c>
+      <c r="J36" t="s">
+        <v>75</v>
+      </c>
+      <c r="K36" t="str">
+        <f t="shared" si="2"/>
+        <v>'#soc_dist': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>52</v>
+      </c>
+      <c r="J37" t="s">
+        <v>76</v>
+      </c>
+      <c r="K37" t="str">
+        <f t="shared" si="2"/>
+        <v>'#lockdown': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
+    <row r="38" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>53</v>
+      </c>
+      <c r="J38" t="s">
+        <v>74</v>
+      </c>
+      <c r="K38" t="str">
+        <f t="shared" si="2"/>
+        <v>'#curfew': 'South Asia',</v>
+      </c>
+    </row>
+    <row r="39" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>54</v>
+      </c>
+      <c r="J39" t="s">
+        <v>75</v>
+      </c>
+      <c r="K39" t="str">
+        <f t="shared" si="2"/>
+        <v>'#hygeine': 'Europe &amp; Central Asia',</v>
+      </c>
+    </row>
+    <row r="40" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I40" t="s">
+        <v>55</v>
+      </c>
+      <c r="J40" t="s">
+        <v>76</v>
+      </c>
+      <c r="K40" t="str">
+        <f t="shared" si="2"/>
+        <v>'#disinfo': 'Latin America &amp; Caribbean',</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>